<commit_message>
Eliminada a planilha 2 por erro
</commit_message>
<xml_diff>
--- a/escolares/os.xlsx
+++ b/escolares/os.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felli\OneDrive\Documentos\planilhas\escolares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03509552-7424-415B-97D4-196AB13AAB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737BAAA9-6111-4881-ADAD-BF3987AEFE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F4C831DD-A057-41D5-87E5-5E01CEC3CEB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F4C831DD-A057-41D5-87E5-5E01CEC3CEB3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="21">
   <si>
     <t>Organização Semanal</t>
   </si>
@@ -85,22 +84,10 @@
     <t>Domir</t>
   </si>
   <si>
-    <t>Sab2</t>
-  </si>
-  <si>
-    <t>Soma</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Soma Acumulada</t>
-  </si>
-  <si>
-    <t>Contagem</t>
-  </si>
-  <si>
     <t>Almoço/Estudos</t>
+  </si>
+  <si>
+    <t>Igreja</t>
   </si>
 </sst>
 </file>
@@ -108,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -169,31 +156,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -223,18 +199,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -253,13 +219,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26164C06-A941-46EB-A436-873DFC208D59}" name="Tabela2" displayName="Tabela2" ref="A2:H10" totalsRowShown="0">
   <autoFilter ref="A2:H10" xr:uid="{26164C06-A941-46EB-A436-873DFC208D59}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D545F91B-2627-4CCC-9083-1FE507391568}" name="Horários" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{D545F91B-2627-4CCC-9083-1FE507391568}" name="Horários" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{79BCBB35-48AC-42F9-8497-C8BCC41FC31E}" name="Dom"/>
     <tableColumn id="3" xr3:uid="{454A5543-6858-4D26-9432-B43B7BB9769D}" name="Seg"/>
     <tableColumn id="4" xr3:uid="{0EB08578-465D-432C-9BAE-1A633741D6DE}" name="Ter"/>
     <tableColumn id="5" xr3:uid="{101DA494-4EEE-4135-927E-2BF5BD51E50B}" name="Qua"/>
-    <tableColumn id="6" xr3:uid="{2A01E153-E7AF-4FDA-B192-361553430BA1}" name="Qui" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{8C0F2317-838C-4B04-8DDB-1B1AF8DE9F34}" name="Sex" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2A01E153-E7AF-4FDA-B192-361553430BA1}" name="Qui" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{8C0F2317-838C-4B04-8DDB-1B1AF8DE9F34}" name="Sex" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{445F8BDE-8AA5-4A2F-96D8-0D3C483546EF}" name="Sab"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -562,25 +528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0C28B-847C-432C-881E-D6096D1183D0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739E8934-0118-4ACB-B20B-70E532939FA1}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +583,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>0.29166666666666669</v>
       </c>
       <c r="B3" t="s">
@@ -657,7 +609,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>0.41666666666666669</v>
       </c>
       <c r="B4" t="s">
@@ -683,7 +635,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>0.5</v>
       </c>
       <c r="B5" t="s">
@@ -699,7 +651,7 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -709,7 +661,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>0.58333333333333337</v>
       </c>
       <c r="B6" t="s">
@@ -724,10 +676,10 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
         <v>13</v>
       </c>
       <c r="H6" t="s">
@@ -735,7 +687,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="B7" t="s">
@@ -750,10 +702,10 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
       <c r="H7" t="s">
@@ -761,11 +713,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>0.75</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -776,10 +728,10 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
@@ -787,11 +739,11 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>0.83333333333333337</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -802,10 +754,10 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>15</v>
       </c>
       <c r="H9" t="s">
@@ -813,7 +765,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>0.875</v>
       </c>
       <c r="B10" t="s">
@@ -828,10 +780,10 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>18</v>
       </c>
       <c r="H10" t="s">
@@ -844,10 +796,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3:H10">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="lastWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(A3,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(A3,0)&lt;(WEEKDAY(TODAY())+7))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(A3,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(A3,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>